<commit_message>
fixed a mistake in 2022 sheet, added 2023 sheet
</commit_message>
<xml_diff>
--- a/Data/DataNotYetUploadedToEDI/Sed_trap/Metals/Digestions/2022_AcidDigestion_EDI.xlsx
+++ b/Data/DataNotYetUploadedToEDI/Sed_trap/Metals/Digestions/2022_AcidDigestion_EDI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cecewood/Documents/Virginia Tech/Sed Traps/2022/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlybauer/Desktop/Reservoirs/Data/DataNotYetUploadedToEDI/Sed_trap/Metals/Digestions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C5BAB76-C775-F942-855C-6B426A5E4BB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AEE31B2-B376-BE40-837A-0B0648E3D934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16940" xr2:uid="{73A57E23-983B-684E-99EC-0D7FD842B02D}"/>
+    <workbookView xWindow="1160" yWindow="500" windowWidth="27640" windowHeight="16000" xr2:uid="{73A57E23-983B-684E-99EC-0D7FD842B02D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1401,9 +1401,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1441,7 +1441,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1547,7 +1547,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1689,7 +1689,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1697,10 +1697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB697616-86FB-0B4D-8F62-1A4E21D2C77E}">
-  <dimension ref="A1:L141"/>
+  <dimension ref="A1:L144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L141"/>
+      <selection activeCell="J144" sqref="J144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2777,8 +2777,8 @@
       <c r="I30" s="4">
         <v>0.01</v>
       </c>
-      <c r="J30" s="4">
-        <v>5.0000000000000001E-3</v>
+      <c r="J30" s="2">
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="K30" s="4">
         <v>0.01</v>
@@ -2813,8 +2813,8 @@
       <c r="I31" s="4">
         <v>0.01</v>
       </c>
-      <c r="J31" s="4">
-        <v>5.0000000000000001E-3</v>
+      <c r="J31" s="2">
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="K31" s="4">
         <v>0.01</v>
@@ -2849,8 +2849,8 @@
       <c r="I32" s="4">
         <v>0.01</v>
       </c>
-      <c r="J32" s="4">
-        <v>5.0000000000000001E-3</v>
+      <c r="J32" s="2">
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="K32" s="4">
         <v>0.01</v>
@@ -3983,8 +3983,8 @@
       <c r="I64" s="4">
         <v>0.01</v>
       </c>
-      <c r="J64" s="4">
-        <v>5.0000000000000001E-3</v>
+      <c r="J64" s="2">
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="K64" s="4">
         <v>0.01</v>
@@ -4019,8 +4019,8 @@
       <c r="I65" s="4">
         <v>0.01</v>
       </c>
-      <c r="J65" s="4">
-        <v>5.0000000000000001E-3</v>
+      <c r="J65" s="2">
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="K65" s="4">
         <v>0.01</v>
@@ -4055,8 +4055,8 @@
       <c r="I66" s="4">
         <v>0.01</v>
       </c>
-      <c r="J66" s="4">
-        <v>5.0000000000000001E-3</v>
+      <c r="J66" s="2">
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="K66" s="4">
         <v>0.01</v>
@@ -5189,8 +5189,8 @@
       <c r="I98" s="4">
         <v>0.01</v>
       </c>
-      <c r="J98" s="4">
-        <v>5.0000000000000001E-3</v>
+      <c r="J98" s="2">
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="K98" s="4">
         <v>0.01</v>
@@ -5225,8 +5225,8 @@
       <c r="I99" s="4">
         <v>0.01</v>
       </c>
-      <c r="J99" s="4">
-        <v>5.0000000000000001E-3</v>
+      <c r="J99" s="2">
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="K99" s="4">
         <v>0.01</v>
@@ -5261,8 +5261,8 @@
       <c r="I100" s="4">
         <v>0.01</v>
       </c>
-      <c r="J100" s="4">
-        <v>5.0000000000000001E-3</v>
+      <c r="J100" s="2">
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="K100" s="4">
         <v>0.01</v>
@@ -6395,8 +6395,8 @@
       <c r="I132" s="4">
         <v>0.01</v>
       </c>
-      <c r="J132" s="4">
-        <v>5.0000000000000001E-3</v>
+      <c r="J132" s="2">
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="K132" s="4">
         <v>0.01</v>
@@ -6431,8 +6431,8 @@
       <c r="I133" s="4">
         <v>0.01</v>
       </c>
-      <c r="J133" s="4">
-        <v>5.0000000000000001E-3</v>
+      <c r="J133" s="2">
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="K133" s="4">
         <v>0.01</v>
@@ -6467,8 +6467,8 @@
       <c r="I134" s="4">
         <v>0.01</v>
       </c>
-      <c r="J134" s="4">
-        <v>5.0000000000000001E-3</v>
+      <c r="J134" s="2">
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="K134" s="4">
         <v>0.01</v>
@@ -6539,8 +6539,8 @@
       <c r="I136" s="4">
         <v>0.01</v>
       </c>
-      <c r="J136" s="4">
-        <v>5.0000000000000001E-3</v>
+      <c r="J136" s="2">
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="K136" s="4">
         <v>0.01</v>
@@ -6575,8 +6575,8 @@
       <c r="I137" s="4">
         <v>0.01</v>
       </c>
-      <c r="J137" s="4">
-        <v>5.0000000000000001E-3</v>
+      <c r="J137" s="2">
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="K137" s="4">
         <v>0.01</v>
@@ -6611,8 +6611,8 @@
       <c r="I138" s="4">
         <v>0.01</v>
       </c>
-      <c r="J138" s="4">
-        <v>5.0000000000000001E-3</v>
+      <c r="J138" s="2">
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="K138" s="4">
         <v>0.01</v>
@@ -6710,6 +6710,9 @@
       <c r="K141" s="1">
         <v>0.01</v>
       </c>
+    </row>
+    <row r="144" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J144" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>